<commit_message>
Verbeterde versie met demo data toegevoegd.
</commit_message>
<xml_diff>
--- a/Input/demo_input_bakkers.xlsx
+++ b/Input/demo_input_bakkers.xlsx
@@ -27,48 +27,102 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="32">
   <si>
     <t>Naam</t>
   </si>
   <si>
-    <t>Inplannen op vrijdag</t>
-  </si>
-  <si>
-    <t>Inplannen op Zaterdag</t>
-  </si>
-  <si>
-    <t>Piet</t>
-  </si>
-  <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Klaas</t>
-  </si>
-  <si>
-    <t>Henk</t>
-  </si>
-  <si>
-    <t>Marie</t>
-  </si>
-  <si>
-    <t>Ellen</t>
-  </si>
-  <si>
-    <t>Joost</t>
-  </si>
-  <si>
-    <t>Floris</t>
-  </si>
-  <si>
-    <t>Maurits</t>
-  </si>
-  <si>
     <t>JA</t>
   </si>
   <si>
     <t>NEE</t>
+  </si>
+  <si>
+    <t>Vrijdag</t>
+  </si>
+  <si>
+    <t>Zaterdag</t>
+  </si>
+  <si>
+    <t>EvenWeken</t>
+  </si>
+  <si>
+    <t>OnevenWeken</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Mila</t>
+  </si>
+  <si>
+    <t>Sophie</t>
+  </si>
+  <si>
+    <t>Zoë</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Tess</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Evi</t>
+  </si>
+  <si>
+    <t>Saar</t>
+  </si>
+  <si>
+    <t>Nora</t>
+  </si>
+  <si>
+    <t>Lieke</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>Yara</t>
+  </si>
+  <si>
+    <t>Liv</t>
+  </si>
+  <si>
+    <t>Noor</t>
+  </si>
+  <si>
+    <t>Eva</t>
+  </si>
+  <si>
+    <t>Lotte</t>
+  </si>
+  <si>
+    <t>Lauren</t>
+  </si>
+  <si>
+    <t>Milou</t>
+  </si>
+  <si>
+    <t>Sofie</t>
+  </si>
+  <si>
+    <t>Maud</t>
+  </si>
+  <si>
+    <t>Nina</t>
+  </si>
+  <si>
+    <t>Nova</t>
+  </si>
+  <si>
+    <t>Sarah</t>
   </si>
 </sst>
 </file>
@@ -132,11 +186,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -414,127 +472,461 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>